<commit_message>
Configuration file updated added more columns
</commit_message>
<xml_diff>
--- a/Configuration.xlsx
+++ b/Configuration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\NETSOL Work\JiraDummy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\JiraRoboticAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906F6689-B8BB-46EF-B543-7240D02F127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E577D666-D814-4C02-AC5D-D2F1E723D006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E66BDAD0-81DF-4A13-B0FB-918E89C30C80}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{E66BDAD0-81DF-4A13-B0FB-918E89C30C80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Status</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Custom field (Application)</t>
+  </si>
+  <si>
+    <t>Customer Reference No</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -432,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C173AF19-D611-49FD-B63C-B737DADB6B61}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,6 +473,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
@@ -512,6 +526,16 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>